<commit_message>
Implemented dynamic property editing
</commit_message>
<xml_diff>
--- a/src/WebMarket/WebMarket/App_Data/Categories.xlsx
+++ b/src/WebMarket/WebMarket/App_Data/Categories.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="63">
   <si>
     <t>Name</t>
   </si>
@@ -52,9 +52,6 @@
     <t>DisplayName</t>
   </si>
   <si>
-    <t>Стабілізатори напруги</t>
-  </si>
-  <si>
     <t>Акумулятори</t>
   </si>
   <si>
@@ -73,13 +70,139 @@
     <t>Реле часу</t>
   </si>
   <si>
-    <t>ББЖ</t>
-  </si>
-  <si>
     <t>Реле напруги</t>
   </si>
   <si>
     <t>Вольтметри</t>
+  </si>
+  <si>
+    <t>TitleList</t>
+  </si>
+  <si>
+    <t>TitleDetails</t>
+  </si>
+  <si>
+    <t>MetaListDescription</t>
+  </si>
+  <si>
+    <t>MetadataDetailsDescription</t>
+  </si>
+  <si>
+    <t>Стабілізотор напруги</t>
+  </si>
+  <si>
+    <t>Стабілізотори напруги, нормалізатори напруги: Phantom, Luxeon, Volter, Вольт, Вольтер</t>
+  </si>
+  <si>
+    <t>Стабілізотор напруги, нормалізатор напруги</t>
+  </si>
+  <si>
+    <t>Акумулятори, батареї: Luxeon, Ventura, B.B. Battery, Vimar, гелеві, кислотно-лужні</t>
+  </si>
+  <si>
+    <t>Акумулятор</t>
+  </si>
+  <si>
+    <t>Акумулятори, батареї: Luxeon, Ventura, Vimar, B.B. battery</t>
+  </si>
+  <si>
+    <t>Акумулятор, батарея</t>
+  </si>
+  <si>
+    <t>Зарядні пристрої: Luxeon</t>
+  </si>
+  <si>
+    <t>Зарядний пристрій</t>
+  </si>
+  <si>
+    <t>Зарядний пристрій, зярядка</t>
+  </si>
+  <si>
+    <t>Перетворювачі напруги, конвертори: Luxeon</t>
+  </si>
+  <si>
+    <t>Перетворювач</t>
+  </si>
+  <si>
+    <t>Перетворювачі напруги: Luxeon</t>
+  </si>
+  <si>
+    <t>Перетворювач, конвертор</t>
+  </si>
+  <si>
+    <t>Реле струму: Энергохит, digitop</t>
+  </si>
+  <si>
+    <t>Реле струму: Енергохіт</t>
+  </si>
+  <si>
+    <t>Реле струму, відсікач</t>
+  </si>
+  <si>
+    <t>Терморегулятори, реле напруги: Энергохит, digitop, одноканальні, двоканальні, триканальні</t>
+  </si>
+  <si>
+    <t>Терморегулятор</t>
+  </si>
+  <si>
+    <t>Терморегулятори: Енергохіт</t>
+  </si>
+  <si>
+    <t>Терморегулятор, термоконтролер</t>
+  </si>
+  <si>
+    <t>Релe часу</t>
+  </si>
+  <si>
+    <t>Реле часу:  Енергохіт</t>
+  </si>
+  <si>
+    <t>Реле часу, відсікач напруги</t>
+  </si>
+  <si>
+    <t>ДБЖ, ББЖ, UPS, блок безперебійного живлення, джерело безперебійного живлення</t>
+  </si>
+  <si>
+    <t>Реле напруги, відсікачі: Энергохит, Volter, digitop, однофазні, трифазні</t>
+  </si>
+  <si>
+    <t>Реле напруги: Енергохіт, Volter, Вольтер</t>
+  </si>
+  <si>
+    <t>Реле напруги, відсікач напруги</t>
+  </si>
+  <si>
+    <t>Вольтметри: Энергохит, digitop</t>
+  </si>
+  <si>
+    <t>Вольтметр</t>
+  </si>
+  <si>
+    <t>Вольтметри:  Енергохіт</t>
+  </si>
+  <si>
+    <t>Стабілізатори (нормалізатори) напруги</t>
+  </si>
+  <si>
+    <t>Джерела безперебійного живлення (ДБЖ), UPS, блоки безперебійного живлення, джерела безперебійного живлення: Luxeon, Вольтер, Вольт</t>
+  </si>
+  <si>
+    <t>Джерела безперебійного живлення (ДБЖ, ББЖ)</t>
+  </si>
+  <si>
+    <t>Стабілізатори (нормалізатори) напруги: Phantom, Volter, Luxeon, Вольт, релейні, симісторні, тиристорні, сервомоторні</t>
+  </si>
+  <si>
+    <t>Джерела безперебійного живлення (ДБЖ, ББЖ): Luxeon, Volter, Вольт, ббж-зарядки, комп'ютерні, інтерактивні, on-line</t>
+  </si>
+  <si>
+    <t>Зарядні пристрої, зарядки: Luxeon</t>
+  </si>
+  <si>
+    <t>Реле часу, таймери: Энергохит, digitop</t>
+  </si>
+  <si>
+    <t>Джерела безперебійного живлення</t>
   </si>
 </sst>
 </file>
@@ -95,12 +218,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -115,8 +244,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,104 +551,239 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.42578125" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="44.7109375" customWidth="1"/>
+    <col min="3" max="3" width="46" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="C3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>